<commit_message>
Add prototype zoom/pan controls
</commit_message>
<xml_diff>
--- a/PlanetaryDataSheet.xlsx
+++ b/PlanetaryDataSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>AstronomicalElement</t>
   </si>
@@ -65,14 +65,20 @@
     <t>Size(km)</t>
   </si>
   <si>
-    <t>DivisibleFactor</t>
+    <t>Divisible Factor of a km</t>
+  </si>
+  <si>
+    <t>RelativeDistance/Factor</t>
+  </si>
+  <si>
+    <t>Uranus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,14 +94,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -118,16 +133,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,237 +425,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="C3" s="3">
-        <f>B3/100</f>
-        <v>10000</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
+      <c r="B5" s="2">
+        <v>1391400</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5/$B$2</f>
+        <v>1391.4</v>
+      </c>
+      <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="E5" s="2">
+        <f>D5/$B$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B6" s="2">
         <v>4879</v>
       </c>
-      <c r="C4" s="3">
-        <f t="shared" ref="C4:C10" si="0">B4/100</f>
-        <v>48.79</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="C6" s="2">
+        <f t="shared" ref="C6:C13" si="0">B6/$B$2</f>
+        <v>4.8789999999999996</v>
+      </c>
+      <c r="D6" s="2">
+        <v>57910000</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E13" si="1">D6/$B$2</f>
+        <v>57910</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B7" s="2">
         <v>12104</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>121.04</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+        <v>12.103999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>108200000</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>108200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B8" s="2">
         <v>12742</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>127.42</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+        <v>12.742000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>149600000</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>149600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B9" s="2">
         <v>6779</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>67.790000000000006</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+        <v>6.7789999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>227900000</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>227900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B10" s="2">
         <v>139822</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>1398.22</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+        <v>139.822</v>
+      </c>
+      <c r="D10" s="2">
+        <v>778600000</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>778600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B11" s="2">
         <v>116464</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>1164.6400000000001</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+        <v>116.464</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1433500000</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>1433500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>50724</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>50.723999999999997</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2872500000</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>2872500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B13" s="2">
         <v>49244</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>492.44</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
+        <v>49.244</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4495100000</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D12/$B$2</f>
+        <v>2872500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="17" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="18" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="19" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="20" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="21" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="22" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>